<commit_message>
add star collection info - in progress
</commit_message>
<xml_diff>
--- a/data/RNAseq_library_metadata.xlsx
+++ b/data/RNAseq_library_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/paper-pycno-sswd-2021-2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48827AA-C961-0547-814E-8D8C7426541A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B94F37D-ECB5-1C42-9DF9-D86B0225243A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35140" windowHeight="20160" xr2:uid="{2887969C-56FD-DD41-9246-1CC715EBAEEB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="160">
   <si>
     <t>library_ID</t>
   </si>
@@ -90,9 +90,6 @@
     <t>H16</t>
   </si>
   <si>
-    <t>second collection</t>
-  </si>
-  <si>
     <t>DallasBank</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>E07</t>
   </si>
   <si>
-    <t>first collection</t>
-  </si>
-  <si>
     <t>E09</t>
   </si>
   <si>
@@ -514,6 +508,9 @@
   </si>
   <si>
     <t>Baby Island</t>
+  </si>
+  <si>
+    <t>Ripple Island or Boulder Reef</t>
   </si>
 </sst>
 </file>
@@ -535,12 +532,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -555,10 +558,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,7 +880,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -889,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -942,19 +946,19 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44441</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -969,19 +973,19 @@
         <v>44462</v>
       </c>
       <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
       </c>
       <c r="O2">
         <v>2</v>
@@ -996,24 +1000,24 @@
         <v>44463</v>
       </c>
       <c r="S2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44441</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3">
         <v>19</v>
@@ -1028,19 +1032,19 @@
         <v>44465</v>
       </c>
       <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
       </c>
       <c r="M3">
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -1055,24 +1059,24 @@
         <v>44466</v>
       </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44441</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>18</v>
@@ -1087,19 +1091,19 @@
         <v>44466</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4">
         <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O4">
         <v>2</v>
@@ -1114,24 +1118,24 @@
         <v>44467</v>
       </c>
       <c r="S4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44441</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
       <c r="F5">
         <v>23</v>
@@ -1146,19 +1150,19 @@
         <v>44471</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M5">
         <v>9</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1173,19 +1177,21 @@
         <v>44487</v>
       </c>
       <c r="S5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6">
         <v>21</v>
       </c>
@@ -1199,19 +1205,19 @@
         <v>44471</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6">
         <v>9</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6">
         <v>6</v>
@@ -1226,19 +1232,21 @@
         <v>44472</v>
       </c>
       <c r="S6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7">
         <v>28</v>
       </c>
@@ -1252,19 +1260,19 @@
         <v>44471</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7">
         <v>9</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7">
         <v>9</v>
@@ -1279,19 +1287,21 @@
         <v>44472</v>
       </c>
       <c r="S7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8">
         <v>25</v>
       </c>
@@ -1305,19 +1315,19 @@
         <v>44471</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8">
         <v>9</v>
       </c>
       <c r="N8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -1332,24 +1342,24 @@
         <v>44487</v>
       </c>
       <c r="S8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44441</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
       </c>
       <c r="F9">
         <v>18</v>
@@ -1364,19 +1374,19 @@
         <v>44471</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M9">
         <v>9</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -1391,19 +1401,21 @@
         <v>44471</v>
       </c>
       <c r="S9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10">
         <v>16</v>
       </c>
@@ -1417,19 +1429,19 @@
         <v>44471</v>
       </c>
       <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" t="s">
         <v>26</v>
-      </c>
-      <c r="K10" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" t="s">
-        <v>27</v>
       </c>
       <c r="M10">
         <v>9</v>
       </c>
       <c r="N10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1444,19 +1456,21 @@
         <v>44485</v>
       </c>
       <c r="S10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11">
         <v>30</v>
       </c>
@@ -1470,19 +1484,19 @@
         <v>44471</v>
       </c>
       <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" t="s">
         <v>26</v>
-      </c>
-      <c r="K11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" t="s">
-        <v>27</v>
       </c>
       <c r="M11">
         <v>9</v>
       </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1497,19 +1511,21 @@
         <v>44472</v>
       </c>
       <c r="S11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12">
         <v>25</v>
       </c>
@@ -1523,19 +1539,19 @@
         <v>44472</v>
       </c>
       <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" t="s">
         <v>26</v>
-      </c>
-      <c r="K12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" t="s">
-        <v>27</v>
       </c>
       <c r="M12">
         <v>9</v>
       </c>
       <c r="N12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1550,19 +1566,21 @@
         <v>44487</v>
       </c>
       <c r="S12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
       <c r="F13">
         <v>20</v>
       </c>
@@ -1576,19 +1594,19 @@
         <v>44472</v>
       </c>
       <c r="J13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13">
         <v>10</v>
       </c>
       <c r="N13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -1603,18 +1621,24 @@
         <v>44474</v>
       </c>
       <c r="S13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44406</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
       </c>
       <c r="F14">
         <v>14</v>
@@ -1629,19 +1653,19 @@
         <v>44476</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M14">
         <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1656,18 +1680,24 @@
         <v>44487</v>
       </c>
       <c r="S14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44406</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
       </c>
       <c r="F15">
         <v>25</v>
@@ -1682,19 +1712,19 @@
         <v>44476</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M15">
         <v>12</v>
       </c>
       <c r="N15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -1709,18 +1739,24 @@
         <v>44487</v>
       </c>
       <c r="S15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44439</v>
+      </c>
+      <c r="E16" t="s">
+        <v>159</v>
       </c>
       <c r="F16">
         <v>17</v>
@@ -1735,19 +1771,19 @@
         <v>44483</v>
       </c>
       <c r="J16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M16">
         <v>9</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1762,24 +1798,24 @@
         <v>44487</v>
       </c>
       <c r="S16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
+        <v>139</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44406</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17">
         <v>16</v>
@@ -1794,19 +1830,19 @@
         <v>44487</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M17">
         <v>13</v>
       </c>
       <c r="N17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1821,18 +1857,24 @@
         <v>44487</v>
       </c>
       <c r="S17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44439</v>
+      </c>
+      <c r="E18" t="s">
+        <v>159</v>
       </c>
       <c r="F18">
         <v>13</v>
@@ -1847,19 +1889,19 @@
         <v>44484</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M18">
         <v>10</v>
       </c>
       <c r="N18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1874,21 +1916,24 @@
         <v>44487</v>
       </c>
       <c r="S18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44425</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F19">
         <v>16</v>
@@ -1903,19 +1948,19 @@
         <v>44483</v>
       </c>
       <c r="J19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M19">
         <v>9</v>
       </c>
       <c r="N19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O19">
         <v>2</v>
@@ -1930,19 +1975,21 @@
         <v>44485</v>
       </c>
       <c r="S19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="F20">
         <v>26</v>
       </c>
@@ -1956,19 +2003,19 @@
         <v>44486</v>
       </c>
       <c r="J20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M20">
         <v>12</v>
       </c>
       <c r="N20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1983,19 +2030,21 @@
         <v>44487</v>
       </c>
       <c r="S20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21">
         <v>23</v>
       </c>
@@ -2009,19 +2058,19 @@
         <v>44483</v>
       </c>
       <c r="J21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M21">
         <v>9</v>
       </c>
       <c r="N21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -2036,21 +2085,24 @@
         <v>44485</v>
       </c>
       <c r="S21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44425</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F22">
         <v>15</v>
@@ -2065,19 +2117,19 @@
         <v>44483</v>
       </c>
       <c r="J22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M22">
         <v>9</v>
       </c>
       <c r="N22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -2092,19 +2144,21 @@
         <v>44487</v>
       </c>
       <c r="S22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
       <c r="F23">
         <v>12</v>
       </c>
@@ -2118,19 +2172,19 @@
         <v>44483</v>
       </c>
       <c r="J23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M23">
         <v>9</v>
       </c>
       <c r="N23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -2145,19 +2199,21 @@
         <v>44487</v>
       </c>
       <c r="S23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
       <c r="F24">
         <v>25</v>
       </c>
@@ -2171,19 +2227,19 @@
         <v>44484</v>
       </c>
       <c r="J24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M24">
         <v>10</v>
       </c>
       <c r="N24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -2198,18 +2254,24 @@
         <v>44487</v>
       </c>
       <c r="S24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44439</v>
+      </c>
+      <c r="E25" t="s">
+        <v>159</v>
       </c>
       <c r="F25">
         <v>15</v>
@@ -2224,19 +2286,19 @@
         <v>44484</v>
       </c>
       <c r="J25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M25">
         <v>10</v>
       </c>
       <c r="N25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O25">
         <v>2</v>
@@ -2251,19 +2313,21 @@
         <v>44485</v>
       </c>
       <c r="S25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26">
         <v>16</v>
       </c>
@@ -2277,25 +2341,25 @@
         <v>44484</v>
       </c>
       <c r="J26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M26">
         <v>10</v>
       </c>
       <c r="N26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O26">
         <v>4</v>
       </c>
       <c r="P26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2304,18 +2368,24 @@
         <v>44485</v>
       </c>
       <c r="S26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D27" s="1">
+        <v>44439</v>
+      </c>
+      <c r="E27" t="s">
+        <v>159</v>
       </c>
       <c r="F27">
         <v>14</v>
@@ -2330,25 +2400,25 @@
         <v>44484</v>
       </c>
       <c r="J27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M27">
         <v>10</v>
       </c>
       <c r="N27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O27">
         <v>14</v>
       </c>
       <c r="P27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -2357,19 +2427,21 @@
         <v>44484</v>
       </c>
       <c r="S27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="F28">
         <v>25</v>
       </c>
@@ -2383,19 +2455,19 @@
         <v>44485</v>
       </c>
       <c r="J28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M28">
         <v>11</v>
       </c>
       <c r="N28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -2410,18 +2482,24 @@
         <v>44487</v>
       </c>
       <c r="S28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D29" s="1">
+        <v>44406</v>
+      </c>
+      <c r="E29" t="s">
+        <v>19</v>
       </c>
       <c r="F29">
         <v>24</v>
@@ -2436,19 +2514,19 @@
         <v>44485</v>
       </c>
       <c r="J29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M29">
         <v>11</v>
       </c>
       <c r="N29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -2463,19 +2541,21 @@
         <v>44487</v>
       </c>
       <c r="S29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="F30">
         <v>25</v>
       </c>
@@ -2489,19 +2569,19 @@
         <v>44483</v>
       </c>
       <c r="J30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M30">
         <v>9</v>
       </c>
       <c r="N30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -2516,19 +2596,21 @@
         <v>44487</v>
       </c>
       <c r="S30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
       <c r="F31">
         <v>25</v>
       </c>
@@ -2542,19 +2624,19 @@
         <v>44486</v>
       </c>
       <c r="J31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M31">
         <v>12</v>
       </c>
       <c r="N31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O31">
         <v>1</v>
@@ -2569,19 +2651,21 @@
         <v>44487</v>
       </c>
       <c r="S31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
       <c r="F32">
         <v>25</v>
       </c>
@@ -2595,19 +2679,19 @@
         <v>44484</v>
       </c>
       <c r="J32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M32">
         <v>10</v>
       </c>
       <c r="N32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -2622,18 +2706,24 @@
         <v>44487</v>
       </c>
       <c r="S32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D33" s="1">
+        <v>44406</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
       </c>
       <c r="F33">
         <v>15</v>
@@ -2648,19 +2738,19 @@
         <v>44487</v>
       </c>
       <c r="J33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M33">
         <v>13</v>
       </c>
       <c r="N33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -2675,1031 +2765,1031 @@
         <v>44487</v>
       </c>
       <c r="S33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B34">
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D34" s="1">
         <v>44708</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B35">
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1">
         <v>44708</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B36">
         <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D36" s="1">
         <v>44708</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B37">
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D37" s="1">
         <v>44708</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D38" s="1">
         <v>44708</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D39" s="1">
         <v>44708</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B40">
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D40" s="1">
         <v>44708</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B41">
         <v>23</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D41" s="1">
         <v>44708</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B42">
         <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D42" s="1">
         <v>44715</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M42">
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B43">
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D43" s="1">
         <v>44715</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B44">
         <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D44" s="1">
         <v>44715</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M44">
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D45" s="1">
         <v>44715</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:19">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B46">
         <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D46" s="1">
         <v>44708</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J46" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M46">
         <v>8</v>
       </c>
       <c r="N46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B47">
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D47" s="1">
         <v>44708</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M47">
         <v>8</v>
       </c>
       <c r="N47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B48">
         <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D48" s="1">
         <v>44708</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J48" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L48" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M48">
         <v>9</v>
       </c>
       <c r="N48" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B49">
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D49" s="1">
         <v>44708</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J49" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M49">
         <v>10</v>
       </c>
       <c r="N49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B50">
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D50" s="1">
         <v>44715</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M50">
         <v>11</v>
       </c>
       <c r="N50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B51">
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D51" s="1">
         <v>44708</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M51">
         <v>11</v>
       </c>
       <c r="N51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B52">
         <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D52" s="1">
         <v>44715</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J52" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M52">
         <v>11</v>
       </c>
       <c r="N52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B53">
         <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D53" s="1">
         <v>44715</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M53">
         <v>11</v>
       </c>
       <c r="N53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B54">
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D54" s="1">
         <v>44708</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M54">
         <v>11</v>
       </c>
       <c r="N54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B55">
         <v>38</v>
       </c>
       <c r="C55" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D55" s="1">
         <v>44715</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L55" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M55">
         <v>12</v>
       </c>
       <c r="N55" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D56" s="1">
         <v>44708</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M56">
         <v>12</v>
       </c>
       <c r="N56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B57">
         <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D57" s="1">
         <v>44708</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M57">
         <v>12</v>
       </c>
       <c r="N57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B58">
         <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D58" s="1">
         <v>44708</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J58" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L58" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M58">
         <v>12</v>
       </c>
       <c r="N58" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B59">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D59" s="1">
         <v>44708</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M59">
         <v>13</v>
       </c>
       <c r="N59" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B60">
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D60" s="1">
         <v>44708</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J60" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L60" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M60">
         <v>13</v>
       </c>
       <c r="N60" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:14">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B61">
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D61" s="1">
         <v>44715</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M61">
         <v>14</v>
       </c>
       <c r="N61" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D62" s="1">
         <v>44715</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M62">
         <v>14</v>
       </c>
       <c r="N62" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B63">
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D63" s="1">
         <v>44715</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M63">
         <v>15</v>
       </c>
       <c r="N63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:14">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B64">
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D64" s="1">
         <v>44708</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M64">
         <v>15</v>
       </c>
       <c r="N64" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:14">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B65">
         <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D65" s="1">
         <v>44715</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L65" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M65">
         <v>15</v>
       </c>
       <c r="N65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add experiment c sample dates
</commit_message>
<xml_diff>
--- a/data/RNAseq_library_metadata.xlsx
+++ b/data/RNAseq_library_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/paper-pycno-sswd-2021-2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCDD79B-E399-CA44-AC55-BCE46E1D278A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB1124E-6D4D-C04E-B55C-49CFCEE650F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35140" windowHeight="20160" xr2:uid="{2887969C-56FD-DD41-9246-1CC715EBAEEB}"/>
   </bookViews>
@@ -856,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428226BF-D753-4547-8962-F4513BB27BBA}">
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2766,6 +2766,9 @@
       <c r="H34" s="1">
         <v>44733</v>
       </c>
+      <c r="I34" s="1">
+        <v>44733</v>
+      </c>
       <c r="J34" t="s">
         <v>141</v>
       </c>
@@ -2780,6 +2783,15 @@
       </c>
       <c r="N34" t="s">
         <v>139</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:19">
@@ -2801,6 +2813,9 @@
       <c r="H35" s="1">
         <v>44733</v>
       </c>
+      <c r="I35" s="1">
+        <v>44733</v>
+      </c>
       <c r="J35" t="s">
         <v>141</v>
       </c>
@@ -2815,6 +2830,15 @@
       </c>
       <c r="N35" t="s">
         <v>139</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:19">
@@ -2836,6 +2860,9 @@
       <c r="H36" s="1">
         <v>44733</v>
       </c>
+      <c r="I36" s="1">
+        <v>44733</v>
+      </c>
       <c r="J36" t="s">
         <v>141</v>
       </c>
@@ -2850,6 +2877,15 @@
       </c>
       <c r="N36" t="s">
         <v>139</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:19">
@@ -2871,6 +2907,9 @@
       <c r="H37" s="1">
         <v>44733</v>
       </c>
+      <c r="I37" s="1">
+        <v>44733</v>
+      </c>
       <c r="J37" t="s">
         <v>141</v>
       </c>
@@ -2885,6 +2924,15 @@
       </c>
       <c r="N37" t="s">
         <v>139</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -2906,6 +2954,9 @@
       <c r="H38" s="1">
         <v>44733</v>
       </c>
+      <c r="I38" s="1">
+        <v>44733</v>
+      </c>
       <c r="J38" t="s">
         <v>141</v>
       </c>
@@ -2920,6 +2971,15 @@
       </c>
       <c r="N38" t="s">
         <v>139</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:19">
@@ -2941,6 +3001,9 @@
       <c r="H39" s="1">
         <v>44733</v>
       </c>
+      <c r="I39" s="1">
+        <v>44733</v>
+      </c>
       <c r="J39" t="s">
         <v>141</v>
       </c>
@@ -2955,6 +3018,15 @@
       </c>
       <c r="N39" t="s">
         <v>139</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:19">
@@ -2976,6 +3048,9 @@
       <c r="H40" s="1">
         <v>44733</v>
       </c>
+      <c r="I40" s="1">
+        <v>44733</v>
+      </c>
       <c r="J40" t="s">
         <v>141</v>
       </c>
@@ -2990,6 +3065,15 @@
       </c>
       <c r="N40" t="s">
         <v>139</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -3011,6 +3095,9 @@
       <c r="H41" s="1">
         <v>44733</v>
       </c>
+      <c r="I41" s="1">
+        <v>44733</v>
+      </c>
       <c r="J41" t="s">
         <v>141</v>
       </c>
@@ -3025,6 +3112,15 @@
       </c>
       <c r="N41" t="s">
         <v>139</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:19">
@@ -3046,6 +3142,9 @@
       <c r="H42" s="1">
         <v>44733</v>
       </c>
+      <c r="I42" s="1">
+        <v>44733</v>
+      </c>
       <c r="J42" t="s">
         <v>141</v>
       </c>
@@ -3060,6 +3159,15 @@
       </c>
       <c r="N42" t="s">
         <v>139</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:19">
@@ -3081,6 +3189,9 @@
       <c r="H43" s="1">
         <v>44733</v>
       </c>
+      <c r="I43" s="1">
+        <v>44733</v>
+      </c>
       <c r="J43" t="s">
         <v>141</v>
       </c>
@@ -3095,6 +3206,15 @@
       </c>
       <c r="N43" t="s">
         <v>139</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:19">
@@ -3116,6 +3236,9 @@
       <c r="H44" s="1">
         <v>44733</v>
       </c>
+      <c r="I44" s="1">
+        <v>44733</v>
+      </c>
       <c r="J44" t="s">
         <v>141</v>
       </c>
@@ -3130,6 +3253,15 @@
       </c>
       <c r="N44" t="s">
         <v>139</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:19">
@@ -3151,6 +3283,9 @@
       <c r="H45" s="1">
         <v>44733</v>
       </c>
+      <c r="I45" s="1">
+        <v>44733</v>
+      </c>
       <c r="J45" t="s">
         <v>141</v>
       </c>
@@ -3165,6 +3300,15 @@
       </c>
       <c r="N45" t="s">
         <v>139</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -3186,6 +3330,9 @@
       <c r="H46" s="1">
         <v>44733</v>
       </c>
+      <c r="I46" s="1">
+        <v>44741</v>
+      </c>
       <c r="J46" t="s">
         <v>141</v>
       </c>
@@ -3224,6 +3371,9 @@
       <c r="H47" s="1">
         <v>44733</v>
       </c>
+      <c r="I47" s="1">
+        <v>44741</v>
+      </c>
       <c r="J47" t="s">
         <v>141</v>
       </c>
@@ -3262,6 +3412,9 @@
       <c r="H48" s="1">
         <v>44733</v>
       </c>
+      <c r="I48" s="1">
+        <v>44742</v>
+      </c>
       <c r="J48" t="s">
         <v>141</v>
       </c>
@@ -3297,6 +3450,9 @@
       <c r="H49" s="1">
         <v>44733</v>
       </c>
+      <c r="I49" s="1">
+        <v>44743</v>
+      </c>
       <c r="J49" t="s">
         <v>141</v>
       </c>
@@ -3335,6 +3491,9 @@
       <c r="H50" s="1">
         <v>44733</v>
       </c>
+      <c r="I50" s="1">
+        <v>44744</v>
+      </c>
       <c r="J50" t="s">
         <v>141</v>
       </c>
@@ -3349,6 +3508,15 @@
       </c>
       <c r="N50" t="s">
         <v>139</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:19">
@@ -3370,6 +3538,9 @@
       <c r="H51" s="1">
         <v>44733</v>
       </c>
+      <c r="I51" s="1">
+        <v>44744</v>
+      </c>
       <c r="J51" t="s">
         <v>141</v>
       </c>
@@ -3384,6 +3555,15 @@
       </c>
       <c r="N51" t="s">
         <v>139</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -3405,6 +3585,9 @@
       <c r="H52" s="1">
         <v>44733</v>
       </c>
+      <c r="I52" s="1">
+        <v>44744</v>
+      </c>
       <c r="J52" t="s">
         <v>141</v>
       </c>
@@ -3446,6 +3629,9 @@
       <c r="H53" s="1">
         <v>44733</v>
       </c>
+      <c r="I53" s="1">
+        <v>44744</v>
+      </c>
       <c r="J53" t="s">
         <v>141</v>
       </c>
@@ -3484,6 +3670,9 @@
       <c r="H54" s="1">
         <v>44733</v>
       </c>
+      <c r="I54" s="1">
+        <v>44744</v>
+      </c>
       <c r="J54" t="s">
         <v>141</v>
       </c>
@@ -3519,6 +3708,9 @@
       <c r="H55" s="1">
         <v>44733</v>
       </c>
+      <c r="I55" s="1">
+        <v>44745</v>
+      </c>
       <c r="J55" t="s">
         <v>141</v>
       </c>
@@ -3557,6 +3749,9 @@
       <c r="H56" s="1">
         <v>44733</v>
       </c>
+      <c r="I56" s="1">
+        <v>44745</v>
+      </c>
       <c r="J56" t="s">
         <v>141</v>
       </c>
@@ -3571,6 +3766,15 @@
       </c>
       <c r="N56" t="s">
         <v>139</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:19">
@@ -3592,6 +3796,9 @@
       <c r="H57" s="1">
         <v>44733</v>
       </c>
+      <c r="I57" s="1">
+        <v>44745</v>
+      </c>
       <c r="J57" t="s">
         <v>141</v>
       </c>
@@ -3606,6 +3813,15 @@
       </c>
       <c r="N57" t="s">
         <v>139</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:19">
@@ -3627,6 +3843,9 @@
       <c r="H58" s="1">
         <v>44733</v>
       </c>
+      <c r="I58" s="1">
+        <v>44745</v>
+      </c>
       <c r="J58" t="s">
         <v>141</v>
       </c>
@@ -3662,6 +3881,9 @@
       <c r="H59" s="1">
         <v>44733</v>
       </c>
+      <c r="I59" s="1">
+        <v>44746</v>
+      </c>
       <c r="J59" t="s">
         <v>141</v>
       </c>
@@ -3676,6 +3898,15 @@
       </c>
       <c r="N59" t="s">
         <v>139</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:19">
@@ -3697,6 +3928,9 @@
       <c r="H60" s="1">
         <v>44733</v>
       </c>
+      <c r="I60" s="1">
+        <v>44746</v>
+      </c>
       <c r="J60" t="s">
         <v>141</v>
       </c>
@@ -3735,6 +3969,9 @@
       <c r="H61" s="1">
         <v>44733</v>
       </c>
+      <c r="I61" s="1">
+        <v>44747</v>
+      </c>
       <c r="J61" t="s">
         <v>141</v>
       </c>
@@ -3749,6 +3986,15 @@
       </c>
       <c r="N61" t="s">
         <v>139</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:19">
@@ -3770,6 +4016,9 @@
       <c r="H62" s="1">
         <v>44733</v>
       </c>
+      <c r="I62" s="1">
+        <v>44747</v>
+      </c>
       <c r="J62" t="s">
         <v>141</v>
       </c>
@@ -3805,6 +4054,9 @@
       <c r="H63" s="1">
         <v>44733</v>
       </c>
+      <c r="I63" s="1">
+        <v>44748</v>
+      </c>
       <c r="J63" t="s">
         <v>141</v>
       </c>
@@ -3819,6 +4071,15 @@
       </c>
       <c r="N63" t="s">
         <v>139</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:19">
@@ -3840,6 +4101,9 @@
       <c r="H64" s="1">
         <v>44733</v>
       </c>
+      <c r="I64" s="1">
+        <v>44748</v>
+      </c>
       <c r="J64" t="s">
         <v>141</v>
       </c>
@@ -3878,6 +4142,9 @@
       <c r="H65" s="1">
         <v>44733</v>
       </c>
+      <c r="I65" s="1">
+        <v>44748</v>
+      </c>
       <c r="J65" t="s">
         <v>141</v>
       </c>
@@ -3896,6 +4163,9 @@
       <c r="S65" t="s">
         <v>152</v>
       </c>
+    </row>
+    <row r="66" spans="1:19">
+      <c r="I66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
metadata almost done - need to double check disease signs at sampling
</commit_message>
<xml_diff>
--- a/data/RNAseq_library_metadata.xlsx
+++ b/data/RNAseq_library_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/paper-pycno-sswd-2021-2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB1124E-6D4D-C04E-B55C-49CFCEE650F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA64F30D-C6A1-6A4E-854C-B39581495B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35140" windowHeight="20160" xr2:uid="{2887969C-56FD-DD41-9246-1CC715EBAEEB}"/>
   </bookViews>
@@ -859,7 +859,7 @@
   <dimension ref="A1:S66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add rnaseq library metadata
</commit_message>
<xml_diff>
--- a/data/RNAseq_library_metadata.xlsx
+++ b/data/RNAseq_library_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/paper-pycno-sswd-2021-2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA64F30D-C6A1-6A4E-854C-B39581495B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95190069-0010-5643-83BA-C89BF2AD814B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35140" windowHeight="20160" xr2:uid="{2887969C-56FD-DD41-9246-1CC715EBAEEB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{2887969C-56FD-DD41-9246-1CC715EBAEEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428226BF-D753-4547-8962-F4513BB27BBA}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>

</xml_diff>